<commit_message>
c7n_gcp: (draft) Update configuration description, insert additional parameters to schema.
</commit_message>
<xml_diff>
--- a/samples/setup/add-new-resources.xlsx
+++ b/samples/setup/add-new-resources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3420" windowWidth="16200" windowHeight="24345"/>
+    <workbookView xWindow="0" yWindow="4560" windowWidth="16200" windowHeight="24345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>@resources.register('managed-zone')</t>
   </si>
@@ -305,9 +305,6 @@
   </si>
   <si>
     <t xml:space="preserve">        'delete',</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        state={})</t>
   </si>
   <si>
     <r>
@@ -380,6 +377,54 @@
   </si>
   <si>
     <t>#                'get', {'project': resource_info['project_id']})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        isServing={'type': 'boolean'},</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">policies:
+…
+    actions:
+      - type: delete
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>isServing: true</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">        status={'type': 'string', 'enum': ['pending', 'done']},</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">policies:
+…
+    actions:
+      - type: delete
+     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>status: pending</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -726,7 +771,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -806,7 +851,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -814,7 +859,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -822,7 +867,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -830,7 +875,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -838,10 +883,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -853,7 +898,7 @@
         <v>@ManagedZone.action_registry.register('delete')</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -869,31 +914,39 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>